<commit_message>
Move class to namespace
</commit_message>
<xml_diff>
--- a/CustomerData.xlsx
+++ b/CustomerData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4991645D-33B4-420F-B27C-58DE93C7C1DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A2DA4F-E209-4D40-ADFB-0727A7EB16E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2107" windowWidth="14400" windowHeight="7380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t>R (pu)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -464,6 +464,10 @@
   </si>
   <si>
     <t>Note: the floating bus is used for the case when "no device" is connected.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wL (pu) = 0.1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -858,7 +862,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1074,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1159,7 +1163,7 @@
         <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
         <v>21</v>
@@ -1438,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C2B6E-74BD-40FA-8EB6-D64D8C21837A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1536,7 +1540,7 @@
         <v>4</v>
       </c>
       <c r="G11">
-        <v>0.999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
@@ -1605,7 +1609,7 @@
         <v>4</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
@@ -1709,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1771,102 +1775,6 @@
       </c>
       <c r="G7" s="3" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>0.01</v>
-      </c>
-      <c r="D8">
-        <v>0.3</v>
-      </c>
-      <c r="E8" s="1">
-        <f>(0.00001)/2</f>
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="F8">
-        <v>0.25</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>0.01</v>
-      </c>
-      <c r="D9">
-        <v>0.3</v>
-      </c>
-      <c r="E9" s="1">
-        <f>(0.00001)/2</f>
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="F9">
-        <v>0.35</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0.01</v>
-      </c>
-      <c r="D10">
-        <v>0.3</v>
-      </c>
-      <c r="E10" s="1">
-        <f>(0.00001)/2</f>
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="F10">
-        <v>0.35</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>0.01</v>
-      </c>
-      <c r="D11">
-        <v>0.3</v>
-      </c>
-      <c r="E11" s="1">
-        <f>(0.00001)/2</f>
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="F11">
-        <v>0.05</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revise Class and ODE
</commit_message>
<xml_diff>
--- a/CustomerData.xlsx
+++ b/CustomerData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yg934\GitHub\Power-System-Analysis-Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3787FF23-E313-4CA2-B85B-B7E6A88BE1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8CC32C-832E-4E80-9A6F-06670C0BA6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1500" yWindow="10390" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerFlow" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -118,7 +118,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -476,19 +476,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="164" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -497,7 +497,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -505,7 +505,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -513,7 +513,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -522,7 +522,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -530,7 +530,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -538,7 +538,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -566,7 +566,7 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -581,7 +581,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -865,49 +865,49 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.19921875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10">
       <c r="A7" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
         <v>70</v>
       </c>
@@ -939,7 +939,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>1</v>
       </c>
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1082,60 +1082,60 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.59765625" customWidth="1"/>
-    <col min="3" max="3" width="13.9296875" customWidth="1"/>
-    <col min="4" max="4" width="15.265625" customWidth="1"/>
-    <col min="5" max="5" width="13.796875" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.46484375" customWidth="1"/>
-    <col min="8" max="8" width="22.265625" customWidth="1"/>
-    <col min="9" max="9" width="24.1328125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>84</v>
@@ -1144,14 +1144,14 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9">
       <c r="A10" s="3"/>
       <c r="B10" s="10" t="s">
         <v>76</v>
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>92</v>
@@ -1169,31 +1169,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9">
       <c r="A13" s="3"/>
       <c r="B13" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9">
       <c r="A14" s="3"/>
       <c r="B14" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9">
       <c r="A15" s="3"/>
       <c r="B15" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="30">
       <c r="A16" s="3"/>
       <c r="B16" s="8" t="s">
         <v>94</v>
@@ -1220,37 +1220,37 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9">
       <c r="A19" s="3"/>
       <c r="B19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9">
       <c r="A20" s="3"/>
       <c r="B20" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="30">
       <c r="A21" s="3"/>
       <c r="B21" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9">
       <c r="A22" s="3"/>
       <c r="B22" s="6" t="s">
         <v>91</v>
@@ -1260,7 +1260,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9">
       <c r="A23" s="3"/>
       <c r="B23" s="10" t="s">
         <v>76</v>
@@ -1270,7 +1270,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:9" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="30">
       <c r="A24" s="3"/>
       <c r="B24" s="8" t="s">
         <v>96</v>
@@ -1279,7 +1279,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9">
       <c r="A25" s="3"/>
       <c r="B25" s="10" t="s">
         <v>76</v>
@@ -1289,7 +1289,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
         <v>93</v>
@@ -1298,18 +1298,18 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9">
       <c r="A27" s="3"/>
       <c r="B27" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9">
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1376,29 +1376,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB93A31-1E5A-4104-8C10-8E6599437516}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.53125" customWidth="1"/>
-    <col min="3" max="3" width="14.9296875" customWidth="1"/>
-    <col min="4" max="4" width="15.73046875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1446,58 +1446,58 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.06640625" customWidth="1"/>
-    <col min="7" max="7" width="14.796875" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1719,42 +1719,42 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="12.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7">
       <c r="A5" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
         <v>73</v>
       </c>
@@ -1788,26 +1788,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.1328125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>80</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1885,45 +1885,45 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>58</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>59</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>60</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>61</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>49</v>

</xml_diff>